<commit_message>
Challenge: implement Decision tree
</commit_message>
<xml_diff>
--- a/Challenge/factory_process_Conformity KC2  KC12.xlsx
+++ b/Challenge/factory_process_Conformity KC2  KC12.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Mon Drive\ENSAM 3A\UE22 - Robust Design and Big data\Challenge\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loudo\Desktop\Challenge_big_data\Challenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6EE3C1-56E7-4E65-BD32-79E67F24BDC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38266BA3-13D2-4CA2-9F8F-367DDA5E3338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -671,7 +671,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -687,9 +687,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -737,14 +734,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Vérification" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -1030,15 +1020,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO810"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A772" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AE772" sqref="AE772"/>
+    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AN3" sqref="AN3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="38" width="11.5703125" style="7"/>
-    <col min="39" max="40" width="15.7109375" style="7" customWidth="1"/>
+    <col min="1" max="38" width="11.5703125" style="6"/>
+    <col min="39" max="40" width="15.7109375" style="6" customWidth="1"/>
     <col min="41" max="41" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -99866,7 +99856,7 @@
   </sheetData>
   <autoFilter ref="A1:AN810" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="A1:AN810">
-    <cfRule type="containsBlanks" dxfId="1" priority="1">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>